<commit_message>
added appendix; support for balance table; modified covariate description slightly
</commit_message>
<xml_diff>
--- a/gp-covariates-overview.xlsx
+++ b/gp-covariates-overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelkramer/Documents/GitHub/gp-personality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B6845C-1703-D049-9290-7A4B68884BCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9503AA02-F80D-E642-9E37-F6C261A31C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="281">
   <si>
     <t>… treatment assignment</t>
   </si>
@@ -156,15 +156,9 @@
     <t>CESD score (depression)</t>
   </si>
   <si>
-    <t>R*MOBILA / R1MOBILW</t>
-  </si>
-  <si>
     <t>R*JHOURS</t>
   </si>
   <si>
-    <t>Satisfaction with Life Scale (Diener)</t>
-  </si>
-  <si>
     <t>*LB003*</t>
   </si>
   <si>
@@ -294,21 +288,6 @@
     <t>cp*014 - cp*018</t>
   </si>
   <si>
-    <t>cp*021 - cp*066 (every 5)</t>
-  </si>
-  <si>
-    <t>cp*022 - cp*067 (every 5)</t>
-  </si>
-  <si>
-    <t>cp*020 - cp*065 (every 5)</t>
-  </si>
-  <si>
-    <t>cp*023 - cp*068 (every 5)</t>
-  </si>
-  <si>
-    <t>cp*024 - cp*069 (every 5)</t>
-  </si>
-  <si>
     <t>mobility</t>
   </si>
   <si>
@@ -318,15 +297,9 @@
     <t>ch*004</t>
   </si>
   <si>
-    <t>ch*023 / ch*027 / ch*041</t>
-  </si>
-  <si>
     <t>ch*011 - ch*015</t>
   </si>
   <si>
-    <t>Summary of mobility problems (walking, staircase, shopping)</t>
-  </si>
-  <si>
     <t>Depression items from Mental Health Inventory</t>
   </si>
   <si>
@@ -480,27 +453,12 @@
     <t>Years of education</t>
   </si>
   <si>
-    <t>Higher secondary education/preparatory university education, US: senior high school degree (ref: vmbo (intermediate secondary education, US: junior high school))</t>
-  </si>
-  <si>
-    <t>Intermediate vocational education, US: junior college degree (ref: vmbo (intermediate secondary education, US: junior high school))</t>
-  </si>
-  <si>
-    <t>Higher vocational education, US: college degree (ref: vmbo (intermediate secondary education, US: junior high school))</t>
-  </si>
-  <si>
-    <t>University degree (ref: vmbo (intermediate secondary education, US: junior high school))</t>
-  </si>
-  <si>
     <t>Member of religion/church</t>
   </si>
   <si>
     <t>*B082</t>
   </si>
   <si>
-    <t>Religious attendance</t>
-  </si>
-  <si>
     <t>Not born in the US</t>
   </si>
   <si>
@@ -510,9 +468,6 @@
     <t>Widowed (marital status)</t>
   </si>
   <si>
-    <t>Live together with this partner</t>
-  </si>
-  <si>
     <t>Matching covariates</t>
   </si>
   <si>
@@ -525,12 +480,6 @@
     <t>Number of rooms (in housing unit)</t>
   </si>
   <si>
-    <t>Household income (logarithm; total, respondent &amp; spouse only)</t>
-  </si>
-  <si>
-    <t>Household wealth (logarithm; total, all assets inc. 2nd home)</t>
-  </si>
-  <si>
     <t>Personal net monthly income in Euros (logarithm)</t>
   </si>
   <si>
@@ -540,75 +489,18 @@
     <t>Financial situation of household (scale from 1-5)</t>
   </si>
   <si>
-    <t>How many hours per week do you work on average?</t>
-  </si>
-  <si>
-    <t>Hours worked/week main job (missings replaced with 0 if non-working)</t>
-  </si>
-  <si>
     <t>Working for pay</t>
   </si>
   <si>
     <t>(Grandparenthood questions in LISS were filtered to participants working for pay)</t>
   </si>
   <si>
-    <t>Some difficulty in mobility rated from 0-5 (different for Wave 1)</t>
-  </si>
-  <si>
     <t>Sum of health conditions</t>
   </si>
   <si>
-    <t>Self-report of health - excellent (ref: good - middle category)</t>
-  </si>
-  <si>
-    <t>Self-report of health - very good (ref: good - middle category)</t>
-  </si>
-  <si>
-    <t>Self-report of health - fair (ref: good - middle category)</t>
-  </si>
-  <si>
-    <t>Self-report of health - poor (ref: good - middle category)</t>
-  </si>
-  <si>
-    <t>Count of nonresident kids</t>
-  </si>
-  <si>
     <t>Number of resident children</t>
   </si>
   <si>
-    <t>How many living children do you have in total?</t>
-  </si>
-  <si>
-    <t>cf*455 / cf*036 (recoded to filter out deceased children)</t>
-  </si>
-  <si>
-    <t>cf*456 / cf*037 (recoded to filter out deceased children)</t>
-  </si>
-  <si>
-    <t>cf*457 / cf*038 (recoded to filter out deceased children)</t>
-  </si>
-  <si>
-    <t>cf*458 / cf*039 (recoded to filter out deceased children)</t>
-  </si>
-  <si>
-    <t>cf*068 (recoded to filter out deceased children)</t>
-  </si>
-  <si>
-    <t>cf*069 (recoded to filter out deceased children)</t>
-  </si>
-  <si>
-    <t>cf*070 (recoded to filter out deceased children)</t>
-  </si>
-  <si>
-    <t>cf*083 (recoded to filter out deceased children)</t>
-  </si>
-  <si>
-    <t>cf*084 (recoded to filter out deceased children)</t>
-  </si>
-  <si>
-    <t>cf*085 (recoded to filter out deceased children)</t>
-  </si>
-  <si>
     <t>Number of living-at-home children in household</t>
   </si>
   <si>
@@ -645,15 +537,6 @@
     <t>Third child living at home</t>
   </si>
   <si>
-    <t>KAGENDERBG / KIDID</t>
-  </si>
-  <si>
-    <t>KABYEARBG / KIDID</t>
-  </si>
-  <si>
-    <t>KAEDUC / KIDID</t>
-  </si>
-  <si>
     <t>KIDID</t>
   </si>
   <si>
@@ -666,9 +549,6 @@
     <t>Date of interview - year</t>
   </si>
   <si>
-    <t>Count of waves participated</t>
-  </si>
-  <si>
     <t>wave</t>
   </si>
   <si>
@@ -688,12 +568,6 @@
   </si>
   <si>
     <t>betterhealth</t>
-  </si>
-  <si>
-    <t>Poor/moderate subjective health status (ref: 3 good)</t>
-  </si>
-  <si>
-    <t>Very good/excellent subjective health status (ref: 3 good)</t>
   </si>
   <si>
     <t>*A030 / *XF065_R</t>
@@ -749,15 +623,6 @@
     <t>Related to Big 5 and LS (Diener et al., 2018; Gebauer et al., 2014)</t>
   </si>
   <si>
-    <t>Count of waves participated (with valid personality assessment 2006-2016)</t>
-  </si>
-  <si>
-    <t>Race: black/african american (reference category: white/caucasian)</t>
-  </si>
-  <si>
-    <t>Race: other (reference category: white/caucasian)</t>
-  </si>
-  <si>
     <t>Dutch spoken at home (primarily)</t>
   </si>
   <si>
@@ -879,6 +744,153 @@
   </si>
   <si>
     <t>Health data not availaible in LISS wave 2014</t>
+  </si>
+  <si>
+    <t>Waves participated (2006-2018)</t>
+  </si>
+  <si>
+    <t>Waves participated</t>
+  </si>
+  <si>
+    <t>Satisfaction with Life Scale</t>
+  </si>
+  <si>
+    <t>Number of nonresident kids</t>
+  </si>
+  <si>
+    <t>Self-report of health - excellent (ref: good)</t>
+  </si>
+  <si>
+    <t>Self-report of health - very good (ref: good)</t>
+  </si>
+  <si>
+    <t>Self-report of health - fair (ref: good)</t>
+  </si>
+  <si>
+    <t>Self-report of health - poor (ref: good)</t>
+  </si>
+  <si>
+    <t>Difficulty in mobility rated from 0-5</t>
+  </si>
+  <si>
+    <t>Hours worked/week main job</t>
+  </si>
+  <si>
+    <t>Household wealth (logarithm)</t>
+  </si>
+  <si>
+    <t>Household income (logarithm)</t>
+  </si>
+  <si>
+    <t>Religious attendance: yearly</t>
+  </si>
+  <si>
+    <t>Religious attendance: monthly</t>
+  </si>
+  <si>
+    <t>Religious attendance: weekly</t>
+  </si>
+  <si>
+    <t>Religious attendance: more</t>
+  </si>
+  <si>
+    <t>Race: black/african american (ref.: white)</t>
+  </si>
+  <si>
+    <t>Race: other (ref.: white)</t>
+  </si>
+  <si>
+    <t>KAGENDERBG</t>
+  </si>
+  <si>
+    <t>KABYEARBG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAEDUC </t>
+  </si>
+  <si>
+    <t>KAEDUC</t>
+  </si>
+  <si>
+    <t>R*MOBILA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average work hours per week </t>
+  </si>
+  <si>
+    <t>Number living children</t>
+  </si>
+  <si>
+    <t>Mobility problems (walking, staircase, shopping)</t>
+  </si>
+  <si>
+    <t>Intermediate vocational education</t>
+  </si>
+  <si>
+    <t>Higher vocational education</t>
+  </si>
+  <si>
+    <t>University degree</t>
+  </si>
+  <si>
+    <t>cf*455 / cf*036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cf*455 / cf*036 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cf*068 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cf*069 </t>
+  </si>
+  <si>
+    <t>cf*070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cf*456 / cf*037 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cf*457 / cf*038 </t>
+  </si>
+  <si>
+    <t>cf*458 / cf*039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cf*083 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cf*084 </t>
+  </si>
+  <si>
+    <t>cf*085</t>
+  </si>
+  <si>
+    <t>Poor/moderate health status (ref.: good)</t>
+  </si>
+  <si>
+    <t>Very good/excellent health status (ref.: good)</t>
+  </si>
+  <si>
+    <t>Higher secondary/preparatory university education</t>
+  </si>
+  <si>
+    <t>ch*023/027/041</t>
+  </si>
+  <si>
+    <t>cp*021 - cp*066</t>
+  </si>
+  <si>
+    <t>cp*022 - cp*067</t>
+  </si>
+  <si>
+    <t>cp*020 - cp*065</t>
+  </si>
+  <si>
+    <t>cp*023 - cp*068</t>
+  </si>
+  <si>
+    <t>cp*024 - cp*069</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1113,14 +1125,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1148,15 +1162,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1440,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDE8F99-DDC3-EF45-A6F4-E9D0E6C5F144}">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="D40" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1461,39 +1466,39 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="48"/>
+      <c r="D2" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="50"/>
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="I2" s="48"/>
+      <c r="H2" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="50"/>
       <c r="J2" s="35"/>
-      <c r="K2" s="46" t="s">
-        <v>268</v>
-      </c>
-      <c r="L2" s="46"/>
+      <c r="K2" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="L2" s="48"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -1501,28 +1506,28 @@
         <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>0</v>
@@ -1534,10 +1539,10 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>4</v>
@@ -1546,10 +1551,10 @@
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>4</v>
@@ -1559,7 +1564,7 @@
       </c>
       <c r="J4" s="36"/>
       <c r="K4" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" t="str">
@@ -1568,41 +1573,41 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
-        <v>80</v>
+      <c r="A5" s="39" t="s">
+        <v>78</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="K5" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="L5" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="M5" t="str">
         <f>""</f>
@@ -1610,12 +1615,12 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>21</v>
@@ -1624,10 +1629,10 @@
         <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H6" s="30" t="s">
         <v>21</v>
@@ -1637,10 +1642,10 @@
       </c>
       <c r="J6" s="35"/>
       <c r="K6" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="L6" t="s">
-        <v>225</v>
+        <v>183</v>
       </c>
       <c r="M6" t="str">
         <f>""</f>
@@ -1648,9 +1653,9 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>38</v>
@@ -1662,23 +1667,23 @@
         <v>5</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>151</v>
+        <v>274</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J7" s="35"/>
       <c r="K7" t="s">
-        <v>254</v>
+        <v>209</v>
       </c>
       <c r="L7" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="M7" t="str">
         <f>""</f>
@@ -1686,29 +1691,29 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="4"/>
       <c r="C8" s="19"/>
       <c r="D8" s="5"/>
       <c r="E8" s="7"/>
       <c r="F8" s="4" t="s">
-        <v>152</v>
+        <v>258</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J8" s="35"/>
       <c r="K8" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M8" t="str">
         <f>""</f>
@@ -1716,29 +1721,29 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="50"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="19"/>
       <c r="D9" s="5"/>
       <c r="E9" s="7"/>
       <c r="F9" s="4" t="s">
-        <v>153</v>
+        <v>259</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J9" s="35"/>
       <c r="K9" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M9" t="str">
         <f>""</f>
@@ -1746,29 +1751,29 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="50"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="19"/>
       <c r="D10" s="5"/>
       <c r="E10" s="7"/>
       <c r="F10" s="4" t="s">
-        <v>154</v>
+        <v>260</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I10" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J10" s="35"/>
       <c r="K10" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M10" t="str">
         <f>""</f>
@@ -1776,37 +1781,37 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="50"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="4" t="s">
-        <v>157</v>
+        <v>244</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J11" s="35"/>
       <c r="K11" t="s">
-        <v>239</v>
+        <v>194</v>
       </c>
       <c r="L11" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="M11" t="str">
         <f>""</f>
@@ -1814,18 +1819,18 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="50"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="4" t="s">
-        <v>157</v>
+        <v>245</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="24"/>
@@ -1833,10 +1838,10 @@
       <c r="I12" s="31"/>
       <c r="J12" s="35"/>
       <c r="K12" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M12" t="str">
         <f>""</f>
@@ -1844,18 +1849,18 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="50"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4" t="s">
-        <v>157</v>
+        <v>246</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="24"/>
@@ -1863,10 +1868,10 @@
       <c r="I13" s="7"/>
       <c r="J13" s="35"/>
       <c r="K13" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M13" t="str">
         <f>""</f>
@@ -1874,18 +1879,18 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="50"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4" t="s">
-        <v>157</v>
+        <v>247</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="24"/>
@@ -1893,10 +1898,10 @@
       <c r="I14" s="7"/>
       <c r="J14" s="35"/>
       <c r="K14" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M14" t="str">
         <f>""</f>
@@ -1904,12 +1909,12 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="50"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>28</v>
@@ -1918,23 +1923,23 @@
         <v>28</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>236</v>
+        <v>191</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J15" s="35"/>
       <c r="K15" t="s">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="L15" t="s">
-        <v>271</v>
+        <v>226</v>
       </c>
       <c r="M15" t="str">
         <f>""</f>
@@ -1942,12 +1947,12 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="50"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="4" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>22</v>
@@ -1961,10 +1966,10 @@
       <c r="I16" s="7"/>
       <c r="J16" s="35"/>
       <c r="K16" s="14" t="s">
-        <v>272</v>
+        <v>227</v>
       </c>
       <c r="L16" s="14" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
       <c r="M16" t="str">
         <f>""</f>
@@ -1972,12 +1977,12 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="50"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="4" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>23</v>
@@ -1991,10 +1996,10 @@
       <c r="I17" s="7"/>
       <c r="J17" s="35"/>
       <c r="K17" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M17" t="str">
         <f>""</f>
@@ -2002,12 +2007,12 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="50"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>24</v>
@@ -2016,10 +2021,10 @@
         <v>24</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H18" s="30" t="s">
         <v>24</v>
@@ -2029,10 +2034,10 @@
       </c>
       <c r="J18" s="35"/>
       <c r="K18" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="L18" t="s">
-        <v>241</v>
+        <v>196</v>
       </c>
       <c r="M18" t="str">
         <f>""</f>
@@ -2040,12 +2045,12 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="50"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>25</v>
@@ -2054,10 +2059,10 @@
         <v>25</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H19" s="30" t="s">
         <v>25</v>
@@ -2067,10 +2072,10 @@
       </c>
       <c r="J19" s="35"/>
       <c r="K19" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="L19" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="M19" t="str">
         <f>""</f>
@@ -2078,37 +2083,37 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="51"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="28" t="s">
-        <v>224</v>
+        <v>182</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>223</v>
+        <v>181</v>
       </c>
       <c r="D20" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>83</v>
-      </c>
       <c r="H20" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J20" s="36"/>
       <c r="K20" s="25" t="s">
-        <v>226</v>
+        <v>184</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>243</v>
+        <v>198</v>
       </c>
       <c r="M20" t="str">
         <f>""</f>
@@ -2116,39 +2121,39 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="49" t="s">
-        <v>140</v>
+      <c r="A21" s="39" t="s">
+        <v>131</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J21" s="35"/>
       <c r="K21" t="s">
-        <v>253</v>
+        <v>208</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="M21" t="str">
         <f>""</f>
@@ -2156,18 +2161,18 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="50"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="22" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="24"/>
@@ -2175,10 +2180,10 @@
       <c r="I22" s="7"/>
       <c r="J22" s="35"/>
       <c r="K22" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M22" t="str">
         <f>""</f>
@@ -2186,18 +2191,18 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="22" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="24"/>
@@ -2205,10 +2210,10 @@
       <c r="I23" s="7"/>
       <c r="J23" s="35"/>
       <c r="K23" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M23" t="str">
         <f>""</f>
@@ -2216,37 +2221,37 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="50"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4" t="s">
-        <v>166</v>
+        <v>243</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="J24" s="35"/>
       <c r="K24" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="L24" t="s">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="M24" t="str">
         <f>""</f>
@@ -2254,18 +2259,18 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="50"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4" t="s">
-        <v>167</v>
+        <v>242</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="24"/>
@@ -2273,10 +2278,10 @@
       <c r="I25" s="7"/>
       <c r="J25" s="35"/>
       <c r="K25" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="L25" t="s">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="M25" t="str">
         <f>""</f>
@@ -2284,12 +2289,12 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="50"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="4" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>27</v>
@@ -2298,23 +2303,23 @@
         <v>27</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I26" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J26" s="35"/>
       <c r="K26" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="L26" t="s">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="M26" t="str">
         <f>""</f>
@@ -2322,29 +2327,29 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="50"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="4"/>
       <c r="C27" s="19"/>
       <c r="D27" s="5"/>
       <c r="E27" s="7"/>
       <c r="F27" s="4" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J27" s="35"/>
       <c r="K27" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="L27" t="s">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="M27" t="str">
         <f>""</f>
@@ -2352,12 +2357,12 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="50"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4" t="s">
-        <v>172</v>
+        <v>241</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>13</v>
@@ -2366,10 +2371,10 @@
         <v>13</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>171</v>
+        <v>255</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="H28" s="30" t="s">
         <v>13</v>
@@ -2379,10 +2384,10 @@
       </c>
       <c r="J28" s="35"/>
       <c r="K28" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="M28" t="str">
         <f>""</f>
@@ -2390,31 +2395,31 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="51"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="3" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="F29" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="36"/>
+        <v>115</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="38" t="s">
+        <v>155</v>
+      </c>
       <c r="K29" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="L29" s="25" t="s">
-        <v>247</v>
+        <v>202</v>
       </c>
       <c r="M29" t="str">
         <f>""</f>
@@ -2422,14 +2427,14 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="49" t="s">
-        <v>79</v>
+      <c r="A30" s="39" t="s">
+        <v>77</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>175</v>
+        <v>240</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>12</v>
@@ -2438,25 +2443,25 @@
         <v>12</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>99</v>
+        <v>257</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>97</v>
+        <v>275</v>
       </c>
       <c r="H30" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="J30" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="K30" t="s">
         <v>94</v>
       </c>
-      <c r="I30" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="J30" s="35" t="s">
-        <v>276</v>
-      </c>
-      <c r="K30" t="s">
-        <v>103</v>
-      </c>
       <c r="L30" t="s">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="M30" t="str">
         <f>""</f>
@@ -2464,7 +2469,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="50"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="4" t="s">
         <v>42</v>
       </c>
@@ -2478,23 +2483,23 @@
         <v>11</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I31" s="31" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="J31" s="35"/>
       <c r="K31" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="L31" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
       <c r="M31" t="str">
         <f>""</f>
@@ -2502,9 +2507,9 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="50"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="4" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>39</v>
@@ -2521,10 +2526,10 @@
       <c r="I32" s="7"/>
       <c r="J32" s="35"/>
       <c r="K32" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="L32" t="s">
-        <v>249</v>
+        <v>204</v>
       </c>
       <c r="M32" t="str">
         <f>""</f>
@@ -2532,12 +2537,12 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="50"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="4" t="s">
-        <v>177</v>
+        <v>236</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>29</v>
@@ -2546,23 +2551,23 @@
         <v>29</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>221</v>
+        <v>272</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="I33" s="31" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="J33" s="35"/>
       <c r="K33" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="L33" t="s">
-        <v>249</v>
+        <v>204</v>
       </c>
       <c r="M33" t="str">
         <f>""</f>
@@ -2570,12 +2575,12 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="50"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="4" t="s">
-        <v>178</v>
+        <v>237</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>30</v>
@@ -2584,23 +2589,23 @@
         <v>30</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>222</v>
+        <v>273</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
       <c r="I34" s="31" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
       <c r="J34" s="35"/>
       <c r="K34" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M34" t="str">
         <f>""</f>
@@ -2608,12 +2613,12 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="50"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="4" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>31</v>
@@ -2627,10 +2632,10 @@
       <c r="I35" s="7"/>
       <c r="J35" s="35"/>
       <c r="K35" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M35" t="str">
         <f>""</f>
@@ -2638,12 +2643,12 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="51"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="3" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>32</v>
@@ -2657,10 +2662,10 @@
       <c r="I36" s="6"/>
       <c r="J36" s="36"/>
       <c r="K36" s="13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L36" s="13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M36" t="str">
         <f>""</f>
@@ -2668,11 +2673,11 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="49" t="s">
-        <v>139</v>
+      <c r="A37" s="39" t="s">
+        <v>130</v>
       </c>
       <c r="B37" t="s">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>36</v>
@@ -2682,21 +2687,21 @@
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="4" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>184</v>
+        <v>261</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="9" t="s">
-        <v>251</v>
+        <v>206</v>
       </c>
       <c r="L37" t="s">
-        <v>248</v>
+        <v>203</v>
       </c>
       <c r="M37" t="str">
         <f>""</f>
@@ -2704,9 +2709,9 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="50"/>
+      <c r="A38" s="40"/>
       <c r="B38" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>37</v>
@@ -2716,10 +2721,10 @@
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="4" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H38" s="30" t="s">
         <v>9</v>
@@ -2727,10 +2732,10 @@
       <c r="I38" s="7"/>
       <c r="J38" s="35"/>
       <c r="K38" s="9" t="s">
-        <v>227</v>
+        <v>185</v>
       </c>
       <c r="L38" t="s">
-        <v>248</v>
+        <v>203</v>
       </c>
       <c r="M38" t="str">
         <f>""</f>
@@ -2738,35 +2743,35 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="50"/>
+      <c r="A39" s="40"/>
       <c r="B39" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="4" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>184</v>
+        <v>262</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="35" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M39" t="str">
         <f>""</f>
@@ -2774,35 +2779,35 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="50"/>
+      <c r="A40" s="40"/>
       <c r="B40" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="4" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>184</v>
+        <v>261</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="I40" s="7"/>
       <c r="J40" s="35" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M40" t="str">
         <f>""</f>
@@ -2810,33 +2815,33 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="50"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="4" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>206</v>
+        <v>250</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="4" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>188</v>
+        <v>263</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="35"/>
       <c r="K41" s="14" t="s">
-        <v>255</v>
+        <v>210</v>
       </c>
       <c r="L41" t="s">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="M41" t="str">
         <f>""</f>
@@ -2844,33 +2849,33 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="50"/>
+      <c r="A42" s="40"/>
       <c r="B42" s="4" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>206</v>
+        <v>250</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="4" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>189</v>
+        <v>264</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="35"/>
       <c r="K42" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M42" t="str">
         <f>""</f>
@@ -2878,33 +2883,33 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="50"/>
+      <c r="A43" s="40"/>
       <c r="B43" s="4" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>206</v>
+        <v>250</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="4" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>190</v>
+        <v>265</v>
       </c>
       <c r="H43" s="30" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="35"/>
       <c r="K43" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L43" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M43" t="str">
         <f>""</f>
@@ -2912,35 +2917,35 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="50"/>
+      <c r="A44" s="40"/>
       <c r="B44" s="22" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>207</v>
+        <v>251</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="22" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>185</v>
+        <v>266</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="I44" s="7"/>
       <c r="J44" s="35" t="s">
-        <v>216</v>
+        <v>176</v>
       </c>
       <c r="K44" s="14" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="L44" t="s">
-        <v>256</v>
+        <v>211</v>
       </c>
       <c r="M44" t="str">
         <f>""</f>
@@ -2948,33 +2953,33 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="50"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="22" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>207</v>
+        <v>251</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="22" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>186</v>
+        <v>267</v>
       </c>
       <c r="H45" s="30" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="35"/>
       <c r="K45" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L45" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M45" t="str">
         <f>""</f>
@@ -2982,33 +2987,33 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="50"/>
+      <c r="A46" s="40"/>
       <c r="B46" s="22" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>207</v>
+        <v>251</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="22" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>187</v>
+        <v>268</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="I46" s="7"/>
       <c r="J46" s="35"/>
       <c r="K46" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L46" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M46" t="str">
         <f>""</f>
@@ -3016,15 +3021,15 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A47" s="50"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="4" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>208</v>
+        <v>252</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E47" s="7"/>
       <c r="F47" s="4"/>
@@ -3032,13 +3037,13 @@
       <c r="H47" s="5"/>
       <c r="I47" s="7"/>
       <c r="J47" s="35" t="s">
-        <v>274</v>
+        <v>229</v>
       </c>
       <c r="K47" s="14" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="L47" s="14" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="M47" t="str">
         <f>""</f>
@@ -3046,15 +3051,15 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="50"/>
+      <c r="A48" s="40"/>
       <c r="B48" s="4" t="s">
-        <v>266</v>
+        <v>221</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>208</v>
+        <v>253</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E48" s="7"/>
       <c r="F48" s="4"/>
@@ -3063,10 +3068,10 @@
       <c r="I48" s="7"/>
       <c r="J48" s="35"/>
       <c r="K48" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M48" t="str">
         <f>""</f>
@@ -3074,29 +3079,29 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="50"/>
+      <c r="A49" s="40"/>
       <c r="B49" s="4" t="s">
-        <v>267</v>
+        <v>222</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>208</v>
+        <v>253</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E49" s="7"/>
       <c r="F49" s="4"/>
       <c r="G49" s="24"/>
       <c r="H49" s="30" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="35"/>
       <c r="K49" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M49" t="str">
         <f>""</f>
@@ -3104,27 +3109,27 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="50"/>
+      <c r="A50" s="40"/>
       <c r="B50" s="22"/>
       <c r="C50" s="19"/>
       <c r="D50" s="5"/>
       <c r="E50" s="7"/>
       <c r="F50" s="4" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>191</v>
+        <v>269</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="I50" s="7"/>
       <c r="J50" s="35"/>
       <c r="K50" s="14" t="s">
-        <v>257</v>
+        <v>212</v>
       </c>
       <c r="L50" t="s">
-        <v>261</v>
+        <v>216</v>
       </c>
       <c r="M50" t="str">
         <f>""</f>
@@ -3132,27 +3137,27 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="50"/>
+      <c r="A51" s="40"/>
       <c r="B51" s="22"/>
       <c r="C51" s="19"/>
       <c r="D51" s="5"/>
       <c r="E51" s="7"/>
       <c r="F51" s="4" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>192</v>
+        <v>270</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I51" s="7"/>
       <c r="J51" s="35"/>
       <c r="K51" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L51" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M51" t="str">
         <f>""</f>
@@ -3160,27 +3165,27 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="50"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="22"/>
       <c r="C52" s="19"/>
       <c r="D52" s="5"/>
       <c r="E52" s="7"/>
       <c r="F52" s="4" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>193</v>
+        <v>271</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="I52" s="7"/>
       <c r="J52" s="35"/>
       <c r="K52" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L52" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M52" t="str">
         <f>""</f>
@@ -3188,12 +3193,12 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="50"/>
+      <c r="A53" s="40"/>
       <c r="B53" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D53" s="20" t="s">
         <v>26</v>
@@ -3205,10 +3210,10 @@
       <c r="I53" s="7"/>
       <c r="J53" s="35"/>
       <c r="K53" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="L53" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="M53" t="str">
         <f>""</f>
@@ -3216,9 +3221,9 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="51"/>
+      <c r="A54" s="41"/>
       <c r="B54" s="3" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>35</v>
@@ -3235,10 +3240,10 @@
       <c r="I54" s="6"/>
       <c r="J54" s="36"/>
       <c r="K54" s="1" t="s">
-        <v>228</v>
+        <v>186</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="M54" t="str">
         <f>""</f>
@@ -3246,14 +3251,14 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="49" t="s">
-        <v>138</v>
+      <c r="A55" s="39" t="s">
+        <v>129</v>
       </c>
       <c r="B55" t="s">
-        <v>45</v>
+        <v>234</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D55" s="20" t="s">
         <v>14</v>
@@ -3262,10 +3267,10 @@
         <v>14</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>45</v>
+        <v>234</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H55" s="30" t="s">
         <v>14</v>
@@ -3274,13 +3279,13 @@
         <v>14</v>
       </c>
       <c r="J55" s="35" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="K55" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="M55" t="str">
         <f>""</f>
@@ -3288,12 +3293,12 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="50"/>
+      <c r="A56" s="40"/>
       <c r="B56" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D56" s="20" t="s">
         <v>15</v>
@@ -3302,10 +3307,10 @@
         <v>15</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G56" s="24" t="s">
-        <v>89</v>
+        <v>276</v>
       </c>
       <c r="H56" s="30" t="s">
         <v>15</v>
@@ -3314,13 +3319,13 @@
         <v>15</v>
       </c>
       <c r="J56" s="35" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="K56" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="L56" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="M56" t="str">
         <f>""</f>
@@ -3328,12 +3333,12 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="50"/>
+      <c r="A57" s="40"/>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>16</v>
@@ -3342,10 +3347,10 @@
         <v>16</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>90</v>
+        <v>277</v>
       </c>
       <c r="H57" s="30" t="s">
         <v>16</v>
@@ -3354,13 +3359,13 @@
         <v>16</v>
       </c>
       <c r="J57" s="35" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="K57" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="L57" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="M57" t="str">
         <f>""</f>
@@ -3368,12 +3373,12 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" s="50"/>
+      <c r="A58" s="40"/>
       <c r="B58" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D58" s="20" t="s">
         <v>17</v>
@@ -3382,10 +3387,10 @@
         <v>17</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>91</v>
+        <v>278</v>
       </c>
       <c r="H58" s="30" t="s">
         <v>17</v>
@@ -3394,13 +3399,13 @@
         <v>17</v>
       </c>
       <c r="J58" s="35" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="K58" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="L58" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="M58" t="str">
         <f>""</f>
@@ -3408,12 +3413,12 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="50"/>
+      <c r="A59" s="40"/>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D59" s="20" t="s">
         <v>18</v>
@@ -3422,10 +3427,10 @@
         <v>18</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>92</v>
+        <v>279</v>
       </c>
       <c r="H59" s="30" t="s">
         <v>18</v>
@@ -3434,13 +3439,13 @@
         <v>18</v>
       </c>
       <c r="J59" s="35" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="K59" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="L59" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="M59" t="str">
         <f>""</f>
@@ -3448,12 +3453,12 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" s="51"/>
+      <c r="A60" s="41"/>
       <c r="B60" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>19</v>
@@ -3462,10 +3467,10 @@
         <v>19</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>93</v>
+        <v>280</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>19</v>
@@ -3474,13 +3479,13 @@
         <v>19</v>
       </c>
       <c r="J60" s="36" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="M60" t="str">
         <f>""</f>
@@ -3488,14 +3493,14 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C61" s="23" t="s">
         <v>137</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>146</v>
       </c>
       <c r="D61" s="20" t="s">
         <v>20</v>
@@ -3504,10 +3509,10 @@
         <v>20</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="G61" s="23" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="H61" s="33" t="s">
         <v>20</v>
@@ -3517,10 +3522,10 @@
       </c>
       <c r="J61" s="35"/>
       <c r="K61" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="L61" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="M61" t="str">
         <f>""</f>
@@ -3528,9 +3533,9 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="50"/>
+      <c r="A62" s="40"/>
       <c r="B62" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>34</v>
@@ -3542,23 +3547,23 @@
         <v>6</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="I62" s="31" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="J62" s="35"/>
       <c r="K62" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="L62" t="s">
-        <v>262</v>
+        <v>217</v>
       </c>
       <c r="M62" t="str">
         <f>""</f>
@@ -3632,20 +3637,20 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A29"/>
     <mergeCell ref="A30:A36"/>
     <mergeCell ref="A37:A54"/>
     <mergeCell ref="A61:A62"/>
     <mergeCell ref="A55:A60"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
further manuscript changes; last edits before sending to coauthors
</commit_message>
<xml_diff>
--- a/gp-covariates-overview.xlsx
+++ b/gp-covariates-overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelkramer/Documents/GitHub/gp-personality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9503AA02-F80D-E642-9E37-F6C261A31C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58175567-8FC5-EA4B-ABC6-32469D2E06E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1127,15 +1127,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1162,6 +1153,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1445,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDE8F99-DDC3-EF45-A6F4-E9D0E6C5F144}">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D40" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1466,39 +1466,39 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="47"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="44"/>
       <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="E2" s="50"/>
+      <c r="E2" s="47"/>
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="50"/>
+      <c r="I2" s="47"/>
       <c r="J2" s="35"/>
-      <c r="K2" s="48" t="s">
+      <c r="K2" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="L2" s="48"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -1573,7 +1573,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="48" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1615,7 +1615,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="4" t="s">
         <v>140</v>
       </c>
@@ -1653,7 +1653,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="4" t="s">
         <v>141</v>
       </c>
@@ -1691,7 +1691,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="4"/>
       <c r="C8" s="19"/>
       <c r="D8" s="5"/>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="4"/>
       <c r="C9" s="19"/>
       <c r="D9" s="5"/>
@@ -1751,7 +1751,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="4"/>
       <c r="C10" s="19"/>
       <c r="D10" s="5"/>
@@ -1781,7 +1781,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="4" t="s">
         <v>244</v>
       </c>
@@ -1819,7 +1819,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="4" t="s">
         <v>245</v>
       </c>
@@ -1849,7 +1849,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="40"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="4" t="s">
         <v>246</v>
       </c>
@@ -1879,7 +1879,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="4" t="s">
         <v>247</v>
       </c>
@@ -1909,7 +1909,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="4" t="s">
         <v>144</v>
       </c>
@@ -1947,7 +1947,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="4" t="s">
         <v>248</v>
       </c>
@@ -1977,7 +1977,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="4" t="s">
         <v>249</v>
       </c>
@@ -2007,7 +2007,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="4" t="s">
         <v>145</v>
       </c>
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="40"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="4" t="s">
         <v>146</v>
       </c>
@@ -2083,7 +2083,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="41"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="28" t="s">
         <v>182</v>
       </c>
@@ -2121,7 +2121,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="48" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="22" t="s">
@@ -2161,7 +2161,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="22" t="s">
         <v>150</v>
       </c>
@@ -2191,7 +2191,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="40"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="22" t="s">
         <v>150</v>
       </c>
@@ -2221,7 +2221,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="40"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="4" t="s">
         <v>243</v>
       </c>
@@ -2259,7 +2259,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="40"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="4" t="s">
         <v>242</v>
       </c>
@@ -2289,7 +2289,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="40"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="4" t="s">
         <v>152</v>
       </c>
@@ -2327,7 +2327,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="40"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="4"/>
       <c r="C27" s="19"/>
       <c r="D27" s="5"/>
@@ -2357,7 +2357,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="40"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="4" t="s">
         <v>241</v>
       </c>
@@ -2395,7 +2395,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="41"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="3" t="s">
         <v>154</v>
       </c>
@@ -2427,7 +2427,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="48" t="s">
         <v>77</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -2469,7 +2469,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="4" t="s">
         <v>42</v>
       </c>
@@ -2507,7 +2507,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="40"/>
+      <c r="A32" s="49"/>
       <c r="B32" s="4" t="s">
         <v>156</v>
       </c>
@@ -2537,7 +2537,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="40"/>
+      <c r="A33" s="49"/>
       <c r="B33" s="4" t="s">
         <v>236</v>
       </c>
@@ -2575,7 +2575,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="40"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="4" t="s">
         <v>237</v>
       </c>
@@ -2613,7 +2613,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="40"/>
+      <c r="A35" s="49"/>
       <c r="B35" s="4" t="s">
         <v>238</v>
       </c>
@@ -2643,7 +2643,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="41"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="3" t="s">
         <v>239</v>
       </c>
@@ -2673,7 +2673,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="48" t="s">
         <v>130</v>
       </c>
       <c r="B37" t="s">
@@ -2709,7 +2709,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="40"/>
+      <c r="A38" s="49"/>
       <c r="B38" t="s">
         <v>157</v>
       </c>
@@ -2743,7 +2743,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="40"/>
+      <c r="A39" s="49"/>
       <c r="B39" t="s">
         <v>159</v>
       </c>
@@ -2779,7 +2779,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="40"/>
+      <c r="A40" s="49"/>
       <c r="B40" t="s">
         <v>160</v>
       </c>
@@ -2815,7 +2815,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="40"/>
+      <c r="A41" s="49"/>
       <c r="B41" s="4" t="s">
         <v>161</v>
       </c>
@@ -2849,7 +2849,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="40"/>
+      <c r="A42" s="49"/>
       <c r="B42" s="4" t="s">
         <v>163</v>
       </c>
@@ -2883,7 +2883,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="40"/>
+      <c r="A43" s="49"/>
       <c r="B43" s="4" t="s">
         <v>162</v>
       </c>
@@ -2917,7 +2917,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="40"/>
+      <c r="A44" s="49"/>
       <c r="B44" s="22" t="s">
         <v>164</v>
       </c>
@@ -2953,7 +2953,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="40"/>
+      <c r="A45" s="49"/>
       <c r="B45" s="22" t="s">
         <v>165</v>
       </c>
@@ -2987,7 +2987,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="40"/>
+      <c r="A46" s="49"/>
       <c r="B46" s="22" t="s">
         <v>166</v>
       </c>
@@ -3021,7 +3021,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A47" s="40"/>
+      <c r="A47" s="49"/>
       <c r="B47" s="4" t="s">
         <v>220</v>
       </c>
@@ -3051,7 +3051,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="40"/>
+      <c r="A48" s="49"/>
       <c r="B48" s="4" t="s">
         <v>221</v>
       </c>
@@ -3079,7 +3079,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="40"/>
+      <c r="A49" s="49"/>
       <c r="B49" s="4" t="s">
         <v>222</v>
       </c>
@@ -3109,7 +3109,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="40"/>
+      <c r="A50" s="49"/>
       <c r="B50" s="22"/>
       <c r="C50" s="19"/>
       <c r="D50" s="5"/>
@@ -3137,7 +3137,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="40"/>
+      <c r="A51" s="49"/>
       <c r="B51" s="22"/>
       <c r="C51" s="19"/>
       <c r="D51" s="5"/>
@@ -3165,7 +3165,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="40"/>
+      <c r="A52" s="49"/>
       <c r="B52" s="22"/>
       <c r="C52" s="19"/>
       <c r="D52" s="5"/>
@@ -3193,7 +3193,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="40"/>
+      <c r="A53" s="49"/>
       <c r="B53" t="s">
         <v>171</v>
       </c>
@@ -3221,7 +3221,7 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="41"/>
+      <c r="A54" s="50"/>
       <c r="B54" s="3" t="s">
         <v>172</v>
       </c>
@@ -3251,7 +3251,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="48" t="s">
         <v>129</v>
       </c>
       <c r="B55" t="s">
@@ -3293,7 +3293,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="40"/>
+      <c r="A56" s="49"/>
       <c r="B56" t="s">
         <v>46</v>
       </c>
@@ -3333,7 +3333,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="40"/>
+      <c r="A57" s="49"/>
       <c r="B57" t="s">
         <v>47</v>
       </c>
@@ -3373,7 +3373,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" s="40"/>
+      <c r="A58" s="49"/>
       <c r="B58" t="s">
         <v>48</v>
       </c>
@@ -3413,7 +3413,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="40"/>
+      <c r="A59" s="49"/>
       <c r="B59" t="s">
         <v>49</v>
       </c>
@@ -3453,7 +3453,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" s="41"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="3" t="s">
         <v>50</v>
       </c>
@@ -3493,7 +3493,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="39" t="s">
+      <c r="A61" s="48" t="s">
         <v>128</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -3533,7 +3533,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="40"/>
+      <c r="A62" s="49"/>
       <c r="B62" t="s">
         <v>173</v>
       </c>
@@ -3638,17 +3638,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H2:I2"/>
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A29"/>
     <mergeCell ref="A30:A36"/>
     <mergeCell ref="A37:A54"/>
     <mergeCell ref="A61:A62"/>
     <mergeCell ref="A55:A60"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
first version of Results
</commit_message>
<xml_diff>
--- a/gp-covariates-overview.xlsx
+++ b/gp-covariates-overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelkramer/Documents/GitHub/gp-personality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE0E6CD-E5C6-1147-A01F-2AC6A79F0A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95348FC-C309-024E-9656-64BB0798A596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -772,9 +772,6 @@
     <t>Differential change in life satisfaction for grandparents (Tanskanen, Danielsbacka, Coall, &amp; Jokela, 2019; Di Gessa, Bordone, &amp; Arpino, 2019);  change not clear for Big Five; average Big Five levels also different for men/women (Schmitt et al., 2008; Weisberg et al., 2011); Coall et al. (2018): “maternal grandmothers tend to invest the most in their grandchildren, followed by maternal grandfathers, then paternal grandmothers, with paternal grandfathers investing the least“ (see also Danielsbacka et al., 2011); no gender differences in overall/average life satisfaction (Batz-Barbarich et al., 2018)</t>
   </si>
   <si>
-    <t>Fewer years of education are associated with having more children &amp; having them earlier (which might be passed on to the next generation), earlier childbirth also increases the likelihood of having grandkidssee (Skopek &amp; Leopold, 2017; Götmark &amp; Andersson, 2020) for effect of education/SES on age of first birth (van Roode et al., 2017)</t>
-  </si>
-  <si>
     <t>Conservative religious ideology still associated with having a large family (Hayford &amp; Morgan, 2008); "religiosity, particularly religious beliefs, shows a substantially positive effect on fertility" (Zhang, 2008); in the Netherlands probably not as important; also related to contraceptive use and abortion; religiosity passes down (to a degree) to the child's family; see Götmark &amp; Andersson (2020) for a cross-country perspective</t>
   </si>
   <si>
@@ -784,9 +781,6 @@
     <t>Higher education associated with higher life satisfaction (Salinas-Jiménez et al., 2011; but see Powdthavee et al., 2015); associated with Big Five (Nießen et al., 2020)</t>
   </si>
   <si>
-    <t>Some effects for LS (U-shape? Galambos et al., 2020); small effects for Big Five (Specht et al., 2011); Big 5 development (Donnellan &amp; Lucas, 2008; Soto et al., 2011)</t>
-  </si>
-  <si>
     <t>Immigrant status related to life satisfaction (Safi, 2010); Big Five related to migration intentions (Fouarge et al., 2019) and within-country migration (Jokela, 2009; Jokela et al., 2008)</t>
   </si>
   <si>
@@ -818,9 +812,6 @@
   </si>
   <si>
     <t>Women become grandparents at an earlier age (Leopold &amp; Skopek, 2015a): 2 years earlier for Netherlands and 3 years earlier for USA</t>
-  </si>
-  <si>
-    <t>Higher age associated with an increased likelihood of transition to GP (Margolis &amp; Verdery, 2019; Leopold &amp; Skopek, 2015a)</t>
   </si>
   <si>
     <t>more free time if already retired and not working -&gt; social investment; employed grandparents are less likely to provide care on a regular basis (Hank &amp; Buber, 2009); Economic situation associated with life satisfaction (Jebb, Tay, Diener, &amp; Oishi, 2018); small associations of Big Five with income/wealth, esp. Conscientiousness (Duckworth et al., 2012)</t>
@@ -3969,6 +3960,15 @@
   </si>
   <si>
     <t>Children leaving home associated with Big Five change in parents? -&gt; small negative effect for Extraversion (Beck, 2019; only rank-order statbility effects in Specht et al., 2011 using only SOEP); firstborn child moving out associated with life satisfaction losses, esp. in families with traditional gender roles (Collischon et al., 2021)</t>
+  </si>
+  <si>
+    <t>Fewer years of education are associated with having more children &amp; having them earlier (which might be passed on to the next generation), earlier childbirth also increases the likelihood of having grandkids (see Skopek &amp; Leopold, 2017; Götmark &amp; Andersson, 2020) for effect of education/SES on age of first birth (van Roode et al., 2017)</t>
+  </si>
+  <si>
+    <t>Higher age associated with an increased likelihood of transition to grandparenthood (Margolis &amp; Verdery, 2019; Leopold &amp; Skopek, 2015a)</t>
+  </si>
+  <si>
+    <t>Some effects for life satisfaction (U-shape? Galambos et al., 2020); small effects for Big Five (Specht et al., 2011); Big Five development (Donnellan &amp; Lucas, 2008; Soto et al., 2011)</t>
   </si>
 </sst>
 </file>
@@ -4230,6 +4230,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4256,15 +4265,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4548,8 +4548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDE8F99-DDC3-EF45-A6F4-E9D0E6C5F144}">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4569,39 +4569,39 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="44" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="46"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="49"/>
+      <c r="E2" s="52"/>
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="I2" s="49"/>
+      <c r="I2" s="52"/>
       <c r="J2" s="35"/>
-      <c r="K2" s="47" t="s">
+      <c r="K2" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="L2" s="47"/>
+      <c r="L2" s="50"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -4676,7 +4676,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="41" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -4707,17 +4707,17 @@
         <v>93</v>
       </c>
       <c r="K5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L5" t="s">
         <v>247</v>
       </c>
       <c r="M5" s="40" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="51"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="4" t="s">
         <v>139</v>
       </c>
@@ -4744,10 +4744,10 @@
       </c>
       <c r="J6" s="35"/>
       <c r="K6" t="s">
-        <v>264</v>
+        <v>349</v>
       </c>
       <c r="L6" t="s">
-        <v>252</v>
+        <v>350</v>
       </c>
       <c r="M6" t="str">
         <f>""</f>
@@ -4755,7 +4755,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="51"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="4" t="s">
         <v>140</v>
       </c>
@@ -4782,10 +4782,10 @@
       </c>
       <c r="J7" s="35"/>
       <c r="K7" t="s">
-        <v>248</v>
+        <v>348</v>
       </c>
       <c r="L7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M7" t="str">
         <f>""</f>
@@ -4793,7 +4793,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="51"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="4"/>
       <c r="C8" s="19"/>
       <c r="D8" s="5"/>
@@ -4823,7 +4823,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="51"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="4"/>
       <c r="C9" s="19"/>
       <c r="D9" s="5"/>
@@ -4853,7 +4853,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="51"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="4"/>
       <c r="C10" s="19"/>
       <c r="D10" s="5"/>
@@ -4883,7 +4883,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="51"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="4" t="s">
         <v>209</v>
       </c>
@@ -4910,10 +4910,10 @@
       </c>
       <c r="J11" s="35"/>
       <c r="K11" t="s">
+        <v>248</v>
+      </c>
+      <c r="L11" t="s">
         <v>249</v>
-      </c>
-      <c r="L11" t="s">
-        <v>250</v>
       </c>
       <c r="M11" t="str">
         <f>""</f>
@@ -4921,7 +4921,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="51"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="4" t="s">
         <v>210</v>
       </c>
@@ -4951,7 +4951,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="51"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="4" t="s">
         <v>211</v>
       </c>
@@ -4981,7 +4981,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="51"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="4" t="s">
         <v>212</v>
       </c>
@@ -5011,7 +5011,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="51"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="4" t="s">
         <v>143</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>193</v>
       </c>
       <c r="L15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M15" t="str">
         <f>""</f>
@@ -5049,7 +5049,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="4" t="s">
         <v>213</v>
       </c>
@@ -5079,7 +5079,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="51"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="4" t="s">
         <v>214</v>
       </c>
@@ -5109,7 +5109,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="51"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="4" t="s">
         <v>144</v>
       </c>
@@ -5136,10 +5136,10 @@
       </c>
       <c r="J18" s="35"/>
       <c r="K18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L18" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M18" t="str">
         <f>""</f>
@@ -5147,7 +5147,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="4" t="s">
         <v>145</v>
       </c>
@@ -5174,10 +5174,10 @@
       </c>
       <c r="J19" s="35"/>
       <c r="K19" t="s">
+        <v>252</v>
+      </c>
+      <c r="L19" t="s">
         <v>254</v>
-      </c>
-      <c r="L19" t="s">
-        <v>256</v>
       </c>
       <c r="M19" t="str">
         <f>""</f>
@@ -5185,7 +5185,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="52"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="28" t="s">
         <v>181</v>
       </c>
@@ -5212,10 +5212,10 @@
       </c>
       <c r="J20" s="36"/>
       <c r="K20" s="25" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="M20" t="str">
         <f>""</f>
@@ -5223,7 +5223,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="41" t="s">
         <v>130</v>
       </c>
       <c r="B21" s="22" t="s">
@@ -5255,7 +5255,7 @@
         <v>183</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M21" t="str">
         <f>""</f>
@@ -5263,7 +5263,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="51"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="22" t="s">
         <v>149</v>
       </c>
@@ -5293,7 +5293,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="22" t="s">
         <v>149</v>
       </c>
@@ -5323,7 +5323,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="51"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="4" t="s">
         <v>208</v>
       </c>
@@ -5350,10 +5350,10 @@
       </c>
       <c r="J24" s="35"/>
       <c r="K24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L24" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M24" t="str">
         <f>""</f>
@@ -5361,7 +5361,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="51"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="4" t="s">
         <v>207</v>
       </c>
@@ -5380,10 +5380,10 @@
       <c r="I25" s="7"/>
       <c r="J25" s="35"/>
       <c r="K25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L25" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M25" t="str">
         <f>""</f>
@@ -5391,7 +5391,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="51"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="4" t="s">
         <v>151</v>
       </c>
@@ -5418,10 +5418,10 @@
       </c>
       <c r="J26" s="35"/>
       <c r="K26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L26" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M26" t="str">
         <f>""</f>
@@ -5429,7 +5429,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="51"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="4"/>
       <c r="C27" s="19"/>
       <c r="D27" s="5"/>
@@ -5448,10 +5448,10 @@
       </c>
       <c r="J27" s="35"/>
       <c r="K27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L27" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M27" t="str">
         <f>""</f>
@@ -5459,7 +5459,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="51"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="4" t="s">
         <v>206</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>94</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M28" t="str">
         <f>""</f>
@@ -5497,7 +5497,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="52"/>
+      <c r="A29" s="43"/>
       <c r="B29" s="3" t="s">
         <v>153</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>94</v>
       </c>
       <c r="L29" s="25" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="M29" t="str">
         <f>""</f>
@@ -5529,7 +5529,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="41" t="s">
         <v>77</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -5563,7 +5563,7 @@
         <v>94</v>
       </c>
       <c r="L30" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="M30" t="str">
         <f>""</f>
@@ -5571,7 +5571,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="51"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="4" t="s">
         <v>42</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>94</v>
       </c>
       <c r="L31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="M31" t="str">
         <f>""</f>
@@ -5609,7 +5609,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="51"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="4" t="s">
         <v>155</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>94</v>
       </c>
       <c r="L32" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="M32" t="str">
         <f>""</f>
@@ -5639,7 +5639,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="51"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="4" t="s">
         <v>201</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>94</v>
       </c>
       <c r="L33" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="M33" t="str">
         <f>""</f>
@@ -5677,7 +5677,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="51"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="4" t="s">
         <v>202</v>
       </c>
@@ -5715,7 +5715,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="51"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="4" t="s">
         <v>203</v>
       </c>
@@ -5745,7 +5745,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="52"/>
+      <c r="A36" s="43"/>
       <c r="B36" s="3" t="s">
         <v>204</v>
       </c>
@@ -5775,7 +5775,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="41" t="s">
         <v>129</v>
       </c>
       <c r="B37" t="s">
@@ -5800,10 +5800,10 @@
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L37" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="M37" t="str">
         <f>""</f>
@@ -5811,7 +5811,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="51"/>
+      <c r="A38" s="42"/>
       <c r="B38" t="s">
         <v>156</v>
       </c>
@@ -5834,10 +5834,10 @@
       <c r="I38" s="7"/>
       <c r="J38" s="35"/>
       <c r="K38" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L38" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="M38" t="str">
         <f>""</f>
@@ -5845,7 +5845,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="51"/>
+      <c r="A39" s="42"/>
       <c r="B39" t="s">
         <v>158</v>
       </c>
@@ -5881,7 +5881,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="51"/>
+      <c r="A40" s="42"/>
       <c r="B40" t="s">
         <v>159</v>
       </c>
@@ -5917,7 +5917,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="51"/>
+      <c r="A41" s="42"/>
       <c r="B41" s="4" t="s">
         <v>160</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>184</v>
       </c>
       <c r="L41" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="M41" t="str">
         <f>""</f>
@@ -5951,7 +5951,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="51"/>
+      <c r="A42" s="42"/>
       <c r="B42" s="4" t="s">
         <v>162</v>
       </c>
@@ -5985,7 +5985,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="51"/>
+      <c r="A43" s="42"/>
       <c r="B43" s="4" t="s">
         <v>161</v>
       </c>
@@ -6019,7 +6019,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="51"/>
+      <c r="A44" s="42"/>
       <c r="B44" s="22" t="s">
         <v>163</v>
       </c>
@@ -6044,10 +6044,10 @@
         <v>175</v>
       </c>
       <c r="K44" s="14" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="L44" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="M44" t="str">
         <f>""</f>
@@ -6055,7 +6055,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="51"/>
+      <c r="A45" s="42"/>
       <c r="B45" s="22" t="s">
         <v>164</v>
       </c>
@@ -6089,7 +6089,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="51"/>
+      <c r="A46" s="42"/>
       <c r="B46" s="22" t="s">
         <v>165</v>
       </c>
@@ -6123,7 +6123,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A47" s="51"/>
+      <c r="A47" s="42"/>
       <c r="B47" s="4" t="s">
         <v>188</v>
       </c>
@@ -6140,7 +6140,7 @@
       <c r="I47" s="7"/>
       <c r="J47" s="35"/>
       <c r="K47" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="L47" s="14" t="s">
         <v>246</v>
@@ -6151,7 +6151,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="51"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="4" t="s">
         <v>189</v>
       </c>
@@ -6179,7 +6179,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="51"/>
+      <c r="A49" s="42"/>
       <c r="B49" s="4" t="s">
         <v>190</v>
       </c>
@@ -6209,7 +6209,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="51"/>
+      <c r="A50" s="42"/>
       <c r="B50" s="22"/>
       <c r="C50" s="19"/>
       <c r="D50" s="5"/>
@@ -6229,7 +6229,7 @@
         <v>185</v>
       </c>
       <c r="L50" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="M50" t="str">
         <f>""</f>
@@ -6237,7 +6237,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="51"/>
+      <c r="A51" s="42"/>
       <c r="B51" s="22"/>
       <c r="C51" s="19"/>
       <c r="D51" s="5"/>
@@ -6265,7 +6265,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="51"/>
+      <c r="A52" s="42"/>
       <c r="B52" s="22"/>
       <c r="C52" s="19"/>
       <c r="D52" s="5"/>
@@ -6293,7 +6293,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="51"/>
+      <c r="A53" s="42"/>
       <c r="B53" t="s">
         <v>170</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>94</v>
       </c>
       <c r="L53" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="M53" t="str">
         <f>""</f>
@@ -6321,7 +6321,7 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="52"/>
+      <c r="A54" s="43"/>
       <c r="B54" s="3" t="s">
         <v>171</v>
       </c>
@@ -6340,7 +6340,7 @@
       <c r="I54" s="6"/>
       <c r="J54" s="36"/>
       <c r="K54" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>96</v>
@@ -6351,7 +6351,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="50" t="s">
+      <c r="A55" s="41" t="s">
         <v>128</v>
       </c>
       <c r="B55" t="s">
@@ -6393,7 +6393,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="51"/>
+      <c r="A56" s="42"/>
       <c r="B56" t="s">
         <v>46</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>192</v>
       </c>
       <c r="K56" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="L56" t="s">
         <v>187</v>
@@ -6433,7 +6433,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="51"/>
+      <c r="A57" s="42"/>
       <c r="B57" t="s">
         <v>47</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>192</v>
       </c>
       <c r="K57" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="L57" t="s">
         <v>187</v>
@@ -6473,7 +6473,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" s="51"/>
+      <c r="A58" s="42"/>
       <c r="B58" t="s">
         <v>48</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>192</v>
       </c>
       <c r="K58" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="L58" t="s">
         <v>187</v>
@@ -6513,7 +6513,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="51"/>
+      <c r="A59" s="42"/>
       <c r="B59" t="s">
         <v>49</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>192</v>
       </c>
       <c r="K59" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="L59" t="s">
         <v>187</v>
@@ -6553,7 +6553,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" s="52"/>
+      <c r="A60" s="43"/>
       <c r="B60" s="3" t="s">
         <v>50</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>192</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>187</v>
@@ -6593,7 +6593,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="50" t="s">
+      <c r="A61" s="41" t="s">
         <v>127</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -6633,7 +6633,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="51"/>
+      <c r="A62" s="42"/>
       <c r="B62" t="s">
         <v>172</v>
       </c>
@@ -6738,17 +6738,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A29"/>
     <mergeCell ref="A30:A36"/>
     <mergeCell ref="A37:A54"/>
     <mergeCell ref="A61:A62"/>
     <mergeCell ref="A55:A60"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6760,374 +6760,374 @@
   <dimension ref="A1:A74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="39" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="39" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="39" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A15" s="39" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="39" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="39" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A20" s="39" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="39" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="39" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="39" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A24" s="39" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="39" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A26" s="39" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A27" s="39" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A28" s="39" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="39" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A30" s="39" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A31" s="39" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A32" s="39" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="39" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A34" s="39" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A35" s="39" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A36" s="39" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A37" s="39" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A38" s="39" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A39" s="39" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A40" s="39" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A41" s="39" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A42" s="39" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A43" s="39" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A44" s="39" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A45" s="39" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A46" s="39" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A47" s="39" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A48" s="39" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A49" s="39" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A50" s="39" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A51" s="39" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A52" s="39" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A53" s="39" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A54" s="39" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A55" s="39" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A56" s="39" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A57" s="39" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A58" s="39" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A59" s="39" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A60" s="39" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A61" s="39" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A62" s="39" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A63" s="39" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A64" s="39" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A65" s="39" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A66" s="39" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A67" s="39" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A68" s="39" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A69" s="39" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A70" s="39" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A71" s="39" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A72" s="39" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A73" s="39" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="20" x14ac:dyDescent="0.2">

</xml_diff>